<commit_message>
Add vote stats + Fix vote_agg
</commit_message>
<xml_diff>
--- a/questionnaires/vote_stats.xlsx
+++ b/questionnaires/vote_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1F8105-140E-2547-9050-5FD7FAAE3226}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CF7F3A-BB6D-8F46-9180-13076CB09A3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="1960" windowWidth="24240" windowHeight="12980" xr2:uid="{DA6BDB4D-B9F7-AD4E-A9F5-7B4E440DE823}"/>
+    <workbookView xWindow="5260" yWindow="-15620" windowWidth="24240" windowHeight="12980" xr2:uid="{DA6BDB4D-B9F7-AD4E-A9F5-7B4E440DE823}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="212">
   <si>
     <t>Country</t>
   </si>
@@ -387,9 +387,6 @@
     <t>Trump</t>
   </si>
   <si>
-    <t>Guilherme Boulos</t>
-  </si>
-  <si>
     <t>Fernando Haddad</t>
   </si>
   <si>
@@ -664,6 +661,12 @@
   </si>
   <si>
     <t>Far right</t>
+  </si>
+  <si>
+    <t>Vote_agg</t>
+  </si>
+  <si>
+    <t>Vote_agg_factor</t>
   </si>
 </sst>
 </file>
@@ -687,8 +690,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FF202122"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -762,7 +764,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -770,11 +772,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -784,12 +815,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,16 +1156,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C970A05-595A-EB4B-8BE2-8A61C904B70B}">
   <dimension ref="A1:AU35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft" activeCell="AA31" sqref="AA31:AA34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" style="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1309,39 +1357,39 @@
         <f>81268924/1000/AB20</f>
         <v>0.31559539465235376</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>118</v>
       </c>
       <c r="AE2">
-        <f>617.122/AD20</f>
-        <v>3.8821962830242495E-3</v>
+        <f>31342.051/AD20</f>
+        <v>0.19716683880100933</v>
       </c>
       <c r="AF2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AI2">
         <f>10744779/1000/AH20</f>
         <v>1.1393514287212572E-2</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AK2">
         <f>27053.961/AJ20</f>
         <v>0.14345398084681388</v>
       </c>
       <c r="AL2" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AM2">
         <f>1881.521/AL20</f>
         <v>4.7943039768836349E-2</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AO2">
         <f>3014.609/AN20</f>
@@ -1451,43 +1499,43 @@
         <v>119</v>
       </c>
       <c r="AE3">
-        <f>31342.051/AD20</f>
-        <v>0.19716683880100933</v>
+        <f>1069.578/AD20</f>
+        <v>6.728510304290742E-3</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI3">
         <f>119494885/1000/AH20</f>
         <v>0.12670960282164231</v>
       </c>
       <c r="AJ3" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AK3">
         <f>13570.097/AJ20</f>
         <v>7.1955616226674041E-2</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AM3">
         <f>10026.475/AL20</f>
         <v>0.25548462635614666</v>
       </c>
       <c r="AN3" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AO3">
         <f>5714.034/AN20</f>
         <v>0.16080395193763386</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="14">
         <f>5906875/B20/1000</f>
         <v>0.3003437984709954</v>
       </c>
@@ -1582,15 +1630,15 @@
         <f>1-AC2-AC3</f>
         <v>0.39619756065723222</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AD4" s="8" t="s">
         <v>120</v>
       </c>
       <c r="AE4">
-        <f>1069.578/AD20</f>
-        <v>6.728510304290742E-3</v>
+        <f>13344.371/AD20</f>
+        <v>8.3946881646573268E-2</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AI4">
         <f>22246455/1000/AH20</f>
@@ -1604,14 +1652,14 @@
         <v>5.075895823520149E-2</v>
       </c>
       <c r="AL4" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM4">
         <f>3621.188/AL20</f>
         <v>9.2271497524839194E-2</v>
       </c>
       <c r="AN4" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AO4">
         <f>2532.452/AN20</f>
@@ -1714,32 +1762,32 @@
         <v>121</v>
       </c>
       <c r="AE5">
-        <f>13344.371/AD20</f>
-        <v>8.3946881646573268E-2</v>
+        <f>5096.35/AD20</f>
+        <v>3.2060161567713741E-2</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AI5">
         <f>15647182/1000/AH20</f>
         <v>1.6591908653646147E-2</v>
       </c>
       <c r="AJ5" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AK5">
         <f>12661.792/AJ20</f>
         <v>6.7139317124554926E-2</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AM5">
         <f>588.839/AL20</f>
         <v>1.5004207550403013E-2</v>
       </c>
       <c r="AN5" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AO5">
         <f>2206.216/AN20</f>
@@ -1835,32 +1883,32 @@
         <v>122</v>
       </c>
       <c r="AE6">
-        <f>5096.35/AD20</f>
-        <v>3.2060161567713741E-2</v>
+        <f>1288.95/AD20</f>
+        <v>8.1085375322936266E-3</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AI6">
         <f>24929325/1000/AH20</f>
         <v>2.6434477671254619E-2</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AK6">
         <f>10876.507/AJ20</f>
         <v>5.7672820141133382E-2</v>
       </c>
       <c r="AL6" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM6">
         <f>414.864/AL20</f>
         <v>1.0571150282488754E-2</v>
       </c>
       <c r="AN6" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AO6">
         <f>1306.45/AN20</f>
@@ -1956,18 +2004,18 @@
         <v>123</v>
       </c>
       <c r="AE7">
-        <f>1288.95/AD20</f>
-        <v>8.1085375322936266E-3</v>
+        <f>859.601/AD20</f>
+        <v>5.4075852215346859E-3</v>
       </c>
       <c r="AH7" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AI7">
         <f>15534558/1000/AH20</f>
         <v>1.6472484777819287E-2</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AK7">
         <f>6323.147/AJ20</f>
@@ -1981,7 +2029,7 @@
         <v>0.57872547851728606</v>
       </c>
       <c r="AN7" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AO7">
         <f>784.274/AN20</f>
@@ -2018,7 +2066,7 @@
         <v>0.35458184480209454</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M8">
         <f>1-SUM(M2:M7)</f>
@@ -2066,29 +2114,29 @@
         <f>1-SUM(AA2:AA7)</f>
         <v>0.42845480223042121</v>
       </c>
-      <c r="AD8" s="8" t="s">
+      <c r="AD8" s="5" t="s">
         <v>124</v>
       </c>
       <c r="AE8">
-        <f>859.601/AD20</f>
-        <v>5.4075852215346859E-3</v>
+        <f>2679.745/AD20</f>
+        <v>1.6857762449649857E-2</v>
       </c>
       <c r="AH8" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AI8">
         <f>13877622/1000/AH20</f>
         <v>1.4715508297521567E-2</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AK8">
         <f>17229.789/AJ20</f>
         <v>9.1361180760208993E-2</v>
       </c>
       <c r="AN8" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AO8">
         <f>1141.332/AN20</f>
@@ -2110,7 +2158,7 @@
         <f>7678491/1000/H20</f>
         <v>0.14940177928125561</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="9"/>
       <c r="N9" s="6" t="s">
         <v>72</v>
       </c>
@@ -2139,29 +2187,29 @@
         <f>157.612/X20</f>
         <v>2.6243422680999415E-3</v>
       </c>
-      <c r="AD9" s="5" t="s">
+      <c r="AD9" s="7" t="s">
         <v>125</v>
       </c>
       <c r="AE9">
-        <f>2679.745/AD20</f>
-        <v>1.6857762449649857E-2</v>
+        <f>49277.01/AD20</f>
+        <v>0.30999223015959376</v>
       </c>
       <c r="AH9" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AI9">
         <f>14539946/AH20/1000</f>
         <v>1.5417821295933519E-2</v>
       </c>
       <c r="AJ9" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AK9">
         <f>17594.839/AJ20</f>
         <v>9.3296863143580863E-2</v>
       </c>
       <c r="AN9" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AO9">
         <f>1036.003/AN20</f>
@@ -2183,7 +2231,7 @@
         <f>1695000/1000/H20</f>
         <v>3.2979919606824865E-2</v>
       </c>
-      <c r="J10" s="10"/>
+      <c r="J10" s="9"/>
       <c r="R10" s="5" t="s">
         <v>89</v>
       </c>
@@ -2202,25 +2250,25 @@
         <v>126</v>
       </c>
       <c r="AE10">
-        <f>49277.01/AD20</f>
-        <v>0.30999223015959376</v>
+        <f>1348.323/AD20</f>
+        <v>8.4820417015048985E-3</v>
       </c>
       <c r="AH10" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AI10">
         <f>229075170/1000/AH20</f>
         <v>0.24290599390091211</v>
       </c>
       <c r="AJ10" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AK10">
         <f>11493.663/AJ20</f>
         <v>6.0945297875669054E-2</v>
       </c>
       <c r="AN10" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AO10">
         <f>307.244/AN20</f>
@@ -2249,15 +2297,15 @@
         <f>8450513/1000/R20</f>
         <v>0.27220681385386081</v>
       </c>
-      <c r="AD11" s="7" t="s">
-        <v>127</v>
+      <c r="AD11" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="AE11">
-        <f>1348.323/AD20</f>
-        <v>8.4820417015048985E-3</v>
+        <f>1-SUM(AE2:AE10)</f>
+        <v>0.33124945061583611</v>
       </c>
       <c r="AH11" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AI11">
         <f>12513061/1000/AH20</f>
@@ -2300,15 +2348,8 @@
         <f>1317380/1000/R20</f>
         <v>4.2435271377583725E-2</v>
       </c>
-      <c r="AD12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE12">
-        <f>1-SUM(AE2:AE11)</f>
-        <v>0.32736725433281177</v>
-      </c>
       <c r="AH12" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AI12">
         <f>27241340/1000/AH20</f>
@@ -2331,7 +2372,7 @@
         <v>0.37427256742572212</v>
       </c>
       <c r="AH13" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AI13">
         <f>12858904/1000/AH20</f>
@@ -2340,7 +2381,7 @@
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.2">
       <c r="AH14" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AI14">
         <f>1-SUM(AI2:AI13)</f>
@@ -2348,135 +2389,135 @@
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AH15" s="10"/>
+      <c r="AH15" s="9"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:42" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="H18" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="F18" t="s">
+      <c r="J18" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="P18" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="H18" t="s">
-        <v>158</v>
-      </c>
-      <c r="J18" t="s">
-        <v>159</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="R18" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="N18" t="s">
-        <v>188</v>
-      </c>
-      <c r="P18" t="s">
-        <v>173</v>
-      </c>
-      <c r="R18" t="s">
+      <c r="T18" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="V18" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="T18" t="s">
+      <c r="X18" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="V18" t="s">
+      <c r="Z18" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB18" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD18" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="AH18" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="X18" t="s">
-        <v>168</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>171</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>170</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>169</v>
-      </c>
-      <c r="AH18" t="s">
+      <c r="AJ18" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AL18" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AN18" s="28" t="s">
         <v>165</v>
-      </c>
-      <c r="AN18" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>155</v>
+      <c r="A19" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="B19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" t="s">
         <v>174</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>175</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>176</v>
       </c>
-      <c r="H19" t="s">
-        <v>177</v>
-      </c>
       <c r="J19" t="s">
+        <v>179</v>
+      </c>
+      <c r="L19" t="s">
+        <v>178</v>
+      </c>
+      <c r="N19" t="s">
+        <v>186</v>
+      </c>
+      <c r="P19" t="s">
         <v>180</v>
       </c>
-      <c r="L19" t="s">
-        <v>179</v>
-      </c>
-      <c r="N19" t="s">
-        <v>187</v>
-      </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
         <v>181</v>
       </c>
-      <c r="R19" t="s">
+      <c r="T19" t="s">
         <v>182</v>
       </c>
-      <c r="T19" t="s">
+      <c r="V19" t="s">
         <v>183</v>
       </c>
-      <c r="V19" t="s">
+      <c r="X19" t="s">
         <v>184</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Z19" t="s">
         <v>185</v>
       </c>
-      <c r="Z19" t="s">
-        <v>186</v>
-      </c>
       <c r="AB19" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD19" t="s">
         <v>189</v>
       </c>
-      <c r="AD19" t="s">
-        <v>190</v>
-      </c>
       <c r="AH19" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ19" t="s">
         <v>202</v>
       </c>
-      <c r="AJ19" t="s">
+      <c r="AL19" t="s">
         <v>203</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AN19" t="s">
         <v>204</v>
-      </c>
-      <c r="AN19" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>153</v>
+      <c r="A20" s="16" t="s">
+        <v>152</v>
       </c>
       <c r="B20">
         <v>19667.045000000006</v>
@@ -2536,9 +2577,14 @@
         <v>35534.164000000004</v>
       </c>
     </row>
+    <row r="22" spans="1:42" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="27" t="s">
+        <v>210</v>
+      </c>
+    </row>
     <row r="23" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>206</v>
+      <c r="A23" s="17" t="s">
+        <v>205</v>
       </c>
       <c r="G23" s="4">
         <f>G2</f>
@@ -2564,10 +2610,6 @@
         <f>Y2</f>
         <v>1.9610969215195736E-3</v>
       </c>
-      <c r="AE23" s="4">
-        <f>AE2</f>
-        <v>3.8821962830242495E-3</v>
-      </c>
       <c r="AI23" s="4">
         <f>AI2</f>
         <v>1.1393514287212572E-2</v>
@@ -2578,8 +2620,8 @@
       </c>
     </row>
     <row r="24" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>207</v>
+      <c r="A24" s="18" t="s">
+        <v>206</v>
       </c>
       <c r="B24" s="3">
         <f>C3+C2</f>
@@ -2638,7 +2680,7 @@
         <v>0.31559539465235376</v>
       </c>
       <c r="AE24" s="3">
-        <f>AE3+AE4</f>
+        <f>AE2+AE3</f>
         <v>0.20389534910530008</v>
       </c>
       <c r="AI24" s="3">
@@ -2659,8 +2701,8 @@
       </c>
     </row>
     <row r="25" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>208</v>
+      <c r="A25" s="19" t="s">
+        <v>207</v>
       </c>
       <c r="G25" s="8">
         <f>G6</f>
@@ -2707,7 +2749,7 @@
         <v>6.8851645248582879E-2</v>
       </c>
       <c r="AE25" s="8">
-        <f>SUM(AE5:AE8)</f>
+        <f>SUM(AE4:AE7)</f>
         <v>0.12952316596811531</v>
       </c>
       <c r="AK25" s="8">
@@ -2724,8 +2766,8 @@
       </c>
     </row>
     <row r="26" spans="1:42" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>209</v>
+      <c r="A26" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="B26" s="5">
         <f>C4</f>
@@ -2780,7 +2822,7 @@
         <v>0.26014934419536156</v>
       </c>
       <c r="AE26" s="5">
-        <f>AE9</f>
+        <f>AE8</f>
         <v>1.6857762449649857E-2</v>
       </c>
       <c r="AI26" s="5">
@@ -2801,8 +2843,8 @@
       </c>
     </row>
     <row r="27" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>210</v>
+      <c r="A27" s="21" t="s">
+        <v>209</v>
       </c>
       <c r="D27" s="7">
         <f>E7</f>
@@ -2849,7 +2891,7 @@
         <v>0.28820704469041403</v>
       </c>
       <c r="AE27" s="7">
-        <f>AE10+AE11</f>
+        <f>AE9+AE10</f>
         <v>0.31847427186109867</v>
       </c>
       <c r="AI27" s="7">
@@ -2870,7 +2912,7 @@
       </c>
     </row>
     <row r="28" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="22" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="6">
@@ -2930,8 +2972,8 @@
         <v>0.39619756065723222</v>
       </c>
       <c r="AE28" s="6">
-        <f>AE12</f>
-        <v>0.32736725433281177</v>
+        <f>AE11</f>
+        <v>0.33124945061583611</v>
       </c>
       <c r="AI28" s="6">
         <f>AI14</f>
@@ -2950,678 +2992,683 @@
         <v>0.49224599740126151</v>
       </c>
     </row>
-    <row r="31" spans="1:42" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B31" s="11">
+    <row r="30" spans="1:42" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="B31" s="10">
         <f>B23+B24</f>
         <v>0.31703201980775442</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <f t="shared" ref="C31:AP31" si="0">C23+C24</f>
         <v>0</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="10">
+        <f>D23+D24</f>
+        <v>0.33608454732720389</v>
+      </c>
+      <c r="E31" s="10">
         <f t="shared" si="0"/>
-        <v>0.33608454732720389</v>
-      </c>
-      <c r="E31" s="11">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F31" s="11">
+      <c r="G31" s="10">
+        <f>G23+G24</f>
+        <v>0.3305757458082742</v>
+      </c>
+      <c r="H31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G31" s="11">
+      <c r="I31" s="10">
+        <f>I23+I24</f>
+        <v>0.19414622965581604</v>
+      </c>
+      <c r="J31" s="10">
         <f t="shared" si="0"/>
-        <v>0.3305757458082742</v>
-      </c>
-      <c r="H31" s="11">
+        <v>0</v>
+      </c>
+      <c r="K31" s="10">
+        <f>K23+K24</f>
+        <v>0.27434455381969713</v>
+      </c>
+      <c r="L31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I31" s="11">
+      <c r="M31" s="10">
+        <f>M23+M24</f>
+        <v>0.14300025016758089</v>
+      </c>
+      <c r="N31" s="10">
         <f t="shared" si="0"/>
-        <v>0.19414622965581604</v>
-      </c>
-      <c r="J31" s="11">
+        <v>0</v>
+      </c>
+      <c r="O31" s="10">
+        <f>O23+O24</f>
+        <v>0.1553642183702523</v>
+      </c>
+      <c r="P31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K31" s="11">
-        <f t="shared" si="0"/>
-        <v>0.27434455381969713</v>
-      </c>
-      <c r="L31" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="11">
-        <f t="shared" si="0"/>
-        <v>0.14300025016758089</v>
-      </c>
-      <c r="N31" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O31" s="11">
-        <f t="shared" si="0"/>
-        <v>0.1553642183702523</v>
-      </c>
-      <c r="P31" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="11">
+      <c r="Q31" s="10">
         <f>Q23+Q24</f>
         <v>0.29554736969111872</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S31" s="11">
+      <c r="S31" s="10">
+        <f>S23+S24</f>
+        <v>1.4798744432903289E-2</v>
+      </c>
+      <c r="T31" s="10">
         <f t="shared" si="0"/>
-        <v>1.4798744432903289E-2</v>
-      </c>
-      <c r="T31" s="11">
+        <v>0</v>
+      </c>
+      <c r="U31" s="10">
+        <f>U23+U24</f>
+        <v>0.35560343323724453</v>
+      </c>
+      <c r="V31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U31" s="11">
+      <c r="W31" s="10">
+        <f>W23+W24</f>
+        <v>0.26006864333354085</v>
+      </c>
+      <c r="X31" s="10">
         <f t="shared" si="0"/>
-        <v>0.35560343323724453</v>
-      </c>
-      <c r="V31" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="10">
+        <f>Y23+Y24</f>
+        <v>0.28860550222398551</v>
+      </c>
+      <c r="Z31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W31" s="11">
+      <c r="AA31" s="10">
+        <f>AA23+AA24</f>
+        <v>0.23054390359478097</v>
+      </c>
+      <c r="AB31" s="10">
         <f t="shared" si="0"/>
-        <v>0.26006864333354085</v>
-      </c>
-      <c r="X31" s="11">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="10">
+        <f>AC23+AC24</f>
+        <v>0.31559539465235376</v>
+      </c>
+      <c r="AD31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y31" s="11">
+      <c r="AE31" s="10">
+        <f>AE23+AE24</f>
+        <v>0.20389534910530008</v>
+      </c>
+      <c r="AF31" s="10">
         <f t="shared" si="0"/>
-        <v>0.28860550222398551</v>
-      </c>
-      <c r="Z31" s="11">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA31" s="11">
-        <f>AA24+AA25</f>
-        <v>0.29939554884336383</v>
-      </c>
-      <c r="AB31" s="11">
+      <c r="AH31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC31" s="11">
-        <f t="shared" si="0"/>
-        <v>0.31559539465235376</v>
-      </c>
-      <c r="AD31" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE31" s="11">
-        <f t="shared" si="0"/>
-        <v>0.20777754538832433</v>
-      </c>
-      <c r="AF31" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG31" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AH31" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI31" s="11">
+      <c r="AI31" s="10">
         <f>AI23+AI24</f>
         <v>0.25132494239222086</v>
       </c>
-      <c r="AJ31" s="11">
+      <c r="AJ31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AK31" s="11">
+      <c r="AK31" s="10">
+        <f>AK23+AK24</f>
+        <v>0.14345398084681388</v>
+      </c>
+      <c r="AL31" s="10">
         <f t="shared" si="0"/>
-        <v>0.14345398084681388</v>
-      </c>
-      <c r="AL31" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="10">
+        <f>AM23+AM24</f>
+        <v>0.30342766612498301</v>
+      </c>
+      <c r="AN31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AM31" s="11">
+      <c r="AO31" s="10">
+        <f>AO23+AO24</f>
+        <v>8.4836919196973351E-2</v>
+      </c>
+      <c r="AP31" s="10">
         <f t="shared" si="0"/>
-        <v>0.30342766612498301</v>
-      </c>
-      <c r="AN31" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AO31" s="11">
-        <f t="shared" si="0"/>
-        <v>8.4836919196973351E-2</v>
-      </c>
-      <c r="AP31" s="11">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:42" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B32" s="12">
+    <row r="32" spans="1:42" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32" s="11">
         <f>B25</f>
         <v>0</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="11">
         <f t="shared" ref="C32:AP32" si="1">C25</f>
         <v>0</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="11">
         <f t="shared" si="1"/>
         <v>6.555604440050819E-2</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="11">
         <f t="shared" si="1"/>
         <v>0.16842807974564011</v>
       </c>
-      <c r="J32" s="12">
+      <c r="J32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K32" s="12">
+      <c r="K32" s="11">
         <f t="shared" si="1"/>
         <v>4.6637048401390047E-2</v>
       </c>
-      <c r="L32" s="12">
+      <c r="L32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M32" s="12">
+      <c r="M32" s="11">
         <f t="shared" si="1"/>
         <v>0.21090455527062618</v>
       </c>
-      <c r="N32" s="12">
+      <c r="N32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O32" s="12">
+      <c r="O32" s="11">
         <f t="shared" si="1"/>
         <v>0.16544202112903789</v>
       </c>
-      <c r="P32" s="12">
+      <c r="P32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="12">
+      <c r="Q32" s="11">
         <f>Q25</f>
         <v>9.8063021365250219E-2</v>
       </c>
-      <c r="R32" s="12">
+      <c r="R32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S32" s="12">
+      <c r="S32" s="11">
         <f t="shared" si="1"/>
         <v>0.10155635508276548</v>
       </c>
-      <c r="T32" s="12">
+      <c r="T32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U32" s="12">
+      <c r="U32" s="11">
         <f t="shared" si="1"/>
         <v>0.16116785576462772</v>
       </c>
-      <c r="V32" s="12">
+      <c r="V32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W32" s="12">
+      <c r="W32" s="11">
         <f t="shared" si="1"/>
         <v>4.2685284003412323E-2</v>
       </c>
-      <c r="X32" s="12">
+      <c r="X32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y32" s="12">
+      <c r="Y32" s="11">
         <f t="shared" si="1"/>
         <v>8.3098566104288132E-2</v>
       </c>
-      <c r="Z32" s="12">
+      <c r="Z32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA32" s="12">
-        <f>AA26</f>
-        <v>0.26014934419536156</v>
-      </c>
-      <c r="AB32" s="12">
+      <c r="AA32" s="11">
+        <f>AA25</f>
+        <v>6.8851645248582879E-2</v>
+      </c>
+      <c r="AB32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC32" s="12">
+      <c r="AC32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AD32" s="12">
+      <c r="AD32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE32" s="12">
+      <c r="AE32" s="11">
         <f t="shared" si="1"/>
         <v>0.12952316596811531</v>
       </c>
-      <c r="AF32" s="12">
+      <c r="AF32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AG32" s="12">
+      <c r="AG32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AH32" s="12">
+      <c r="AH32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AI32" s="12">
+      <c r="AI32" s="11">
         <f>AI25</f>
         <v>0</v>
       </c>
-      <c r="AJ32" s="12">
+      <c r="AJ32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AK32" s="12">
+      <c r="AK32" s="11">
         <f t="shared" si="1"/>
         <v>0.12271457446187553</v>
       </c>
-      <c r="AL32" s="12">
+      <c r="AL32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AM32" s="12">
+      <c r="AM32" s="11">
         <f t="shared" si="1"/>
         <v>9.2271497524839194E-2</v>
       </c>
-      <c r="AN32" s="12">
+      <c r="AN32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AO32" s="12">
+      <c r="AO32" s="11">
         <f t="shared" si="1"/>
         <v>0.3529962320205422</v>
       </c>
-      <c r="AP32" s="12">
+      <c r="AP32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:42" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="B33" s="13">
+    <row r="33" spans="1:42" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="B33" s="12">
         <f>B26+B27</f>
         <v>0.3003437984709954</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="12">
         <f t="shared" ref="C33:AP33" si="2">C26+C27</f>
         <v>0</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="12">
         <f t="shared" si="2"/>
         <v>0.21515262378217845</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="12">
         <f t="shared" si="2"/>
         <v>0.33002627930066741</v>
       </c>
-      <c r="H33" s="13">
+      <c r="H33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I33" s="13">
+      <c r="I33" s="12">
         <f t="shared" si="2"/>
         <v>0.3291966655841988</v>
       </c>
-      <c r="J33" s="13">
+      <c r="J33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K33" s="13">
+      <c r="K33" s="12">
         <f t="shared" si="2"/>
         <v>0.32443655297681828</v>
       </c>
-      <c r="L33" s="13">
+      <c r="L33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M33" s="13">
+      <c r="M33" s="12">
         <f t="shared" si="2"/>
         <v>0.23042130146490516</v>
       </c>
-      <c r="N33" s="13">
+      <c r="N33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O33" s="13">
+      <c r="O33" s="12">
         <f t="shared" si="2"/>
         <v>0.18553126727021874</v>
       </c>
-      <c r="P33" s="13">
+      <c r="P33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q33" s="13">
+      <c r="Q33" s="12">
         <f>Q26+Q27</f>
         <v>0.10091391384584453</v>
       </c>
-      <c r="R33" s="13">
+      <c r="R33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S33" s="13">
+      <c r="S33" s="12">
         <f t="shared" si="2"/>
         <v>0.50937233305860907</v>
       </c>
-      <c r="T33" s="13">
+      <c r="T33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U33" s="13">
+      <c r="U33" s="12">
         <f t="shared" si="2"/>
         <v>0.23171341453711378</v>
       </c>
-      <c r="V33" s="13">
+      <c r="V33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W33" s="13">
+      <c r="W33" s="12">
         <f t="shared" si="2"/>
         <v>0.22512844372181418</v>
       </c>
-      <c r="X33" s="13">
+      <c r="X33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y33" s="13">
+      <c r="Y33" s="12">
         <f t="shared" si="2"/>
         <v>0.46174648835707427</v>
       </c>
-      <c r="Z33" s="13">
+      <c r="Z33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA33" s="13">
-        <f>AA27</f>
-        <v>1.2000304730853364E-2</v>
-      </c>
-      <c r="AB33" s="13">
+      <c r="AA33" s="12">
+        <f>AA26+AA27</f>
+        <v>0.2721496489262149</v>
+      </c>
+      <c r="AB33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC33" s="13">
+      <c r="AC33" s="12">
         <f t="shared" si="2"/>
         <v>0.28820704469041403</v>
       </c>
-      <c r="AD33" s="13">
+      <c r="AD33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AE33" s="13">
+      <c r="AE33" s="12">
         <f t="shared" si="2"/>
         <v>0.33533203431074854</v>
       </c>
-      <c r="AF33" s="13">
+      <c r="AF33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AG33" s="13">
+      <c r="AG33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AH33" s="13">
+      <c r="AH33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AI33" s="13">
+      <c r="AI33" s="12">
         <f>AI26+AI27</f>
         <v>0.29869592147550184</v>
       </c>
-      <c r="AJ33" s="13">
+      <c r="AJ33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AK33" s="13">
+      <c r="AK33" s="12">
         <f t="shared" si="2"/>
         <v>0.40394404843391762</v>
       </c>
-      <c r="AL33" s="13">
+      <c r="AL33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AM33" s="13">
+      <c r="AM33" s="12">
         <f t="shared" si="2"/>
         <v>2.5575357832891769E-2</v>
       </c>
-      <c r="AN33" s="13">
+      <c r="AN33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AO33" s="13">
+      <c r="AO33" s="12">
         <f t="shared" si="2"/>
         <v>6.9920851381222865E-2</v>
       </c>
-      <c r="AP33" s="13">
+      <c r="AP33" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:42" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="14" t="s">
+    <row r="34" spans="1:42" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="13">
         <f>B28</f>
         <v>0.38262418172125018</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="13">
         <f t="shared" ref="C34:AP34" si="3">C28</f>
         <v>0</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="13">
         <f t="shared" si="3"/>
         <v>0.44876282889061769</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="13">
         <f t="shared" si="3"/>
         <v>0.27384193049055028</v>
       </c>
-      <c r="H34" s="14">
+      <c r="H34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I34" s="14">
+      <c r="I34" s="13">
         <f t="shared" si="3"/>
         <v>0.30822902501434507</v>
       </c>
-      <c r="J34" s="14">
+      <c r="J34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K34" s="14">
+      <c r="K34" s="13">
         <f t="shared" si="3"/>
         <v>0.35458184480209454</v>
       </c>
-      <c r="L34" s="14">
+      <c r="L34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M34" s="14">
+      <c r="M34" s="13">
         <f t="shared" si="3"/>
         <v>0.41567389309688774</v>
       </c>
-      <c r="N34" s="14">
+      <c r="N34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O34" s="14">
+      <c r="O34" s="13">
         <f t="shared" si="3"/>
         <v>0.49366249323049105</v>
       </c>
-      <c r="P34" s="14">
+      <c r="P34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q34" s="14">
+      <c r="Q34" s="13">
         <f>Q28</f>
         <v>0.50547569509778656</v>
       </c>
-      <c r="R34" s="14">
+      <c r="R34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S34" s="14">
+      <c r="S34" s="13">
         <f t="shared" si="3"/>
         <v>0.37427256742572212</v>
       </c>
-      <c r="T34" s="14">
+      <c r="T34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U34" s="14">
+      <c r="U34" s="13">
         <f t="shared" si="3"/>
         <v>0.25151529646101389</v>
       </c>
-      <c r="V34" s="14">
+      <c r="V34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W34" s="14">
+      <c r="W34" s="13">
         <f t="shared" si="3"/>
         <v>0.47211762894123266</v>
       </c>
-      <c r="X34" s="14">
+      <c r="X34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Y34" s="14">
+      <c r="Y34" s="13">
         <f t="shared" si="3"/>
         <v>0.16654944331465205</v>
       </c>
-      <c r="Z34" s="14">
+      <c r="Z34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AA34" s="14">
+      <c r="AA34" s="13">
         <f>AA28</f>
         <v>0.42845480223042121</v>
       </c>
-      <c r="AB34" s="14">
+      <c r="AB34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AC34" s="14">
+      <c r="AC34" s="13">
         <f t="shared" si="3"/>
         <v>0.39619756065723222</v>
       </c>
-      <c r="AD34" s="14">
+      <c r="AD34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AE34" s="14">
+      <c r="AE34" s="13">
         <f t="shared" si="3"/>
-        <v>0.32736725433281177</v>
-      </c>
-      <c r="AF34" s="14">
+        <v>0.33124945061583611</v>
+      </c>
+      <c r="AF34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AG34" s="14">
+      <c r="AG34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AH34" s="14">
+      <c r="AH34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI34" s="14">
+      <c r="AI34" s="13">
         <f>AI28</f>
         <v>0.44997913613227736</v>
       </c>
-      <c r="AJ34" s="14">
+      <c r="AJ34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AK34" s="14">
+      <c r="AK34" s="13">
         <f t="shared" si="3"/>
         <v>0.32988739625739294</v>
       </c>
-      <c r="AL34" s="14">
+      <c r="AL34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AM34" s="14">
+      <c r="AM34" s="13">
         <f t="shared" si="3"/>
         <v>0.57872547851728606</v>
       </c>
-      <c r="AN34" s="14">
+      <c r="AN34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AO34" s="14">
+      <c r="AO34" s="13">
         <f t="shared" si="3"/>
         <v>0.49224599740126151</v>
       </c>
-      <c r="AP34" s="14">
+      <c r="AP34" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3729,7 +3776,7 @@
       </c>
       <c r="AA35">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="AB35">
         <f t="shared" si="4"/>
@@ -3745,7 +3792,7 @@
       </c>
       <c r="AE35">
         <f t="shared" si="4"/>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="AF35">
         <f t="shared" si="4"/>

</xml_diff>